<commit_message>
TVRs and GRP final updates
</commit_message>
<xml_diff>
--- a/input/ER and CPRP Channels TV and Digital CTV-Mobile CPM.xlsx
+++ b/input/ER and CPRP Channels TV and Digital CTV-Mobile CPM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://insidemedia-my.sharepoint.com/personal/sachin_saurav_groupm_com/Documents/one_pager_integration/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{C97336F4-2DBB-4B12-A0B3-5B991B61E415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D21C7A99-4973-47FC-B9B4-B06FA08D6BBF}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{C97336F4-2DBB-4B12-A0B3-5B991B61E415}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F865C39-27B4-4D19-A133-D9ACE2793A67}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{7B95265E-B700-400F-8AAD-26C4CDD13252}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Digital CTV-Mobile CPM" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CPRP Channels'!$A$1:$F$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'CPRP Channels'!$A$1:$F$80</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'ER Channels'!$B$1:$F$112</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -4034,7 +4034,7 @@
   <dimension ref="A1:F80"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5648,7 +5648,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F79" xr:uid="{58D884C3-B977-47D3-B44D-AB1230B14EE3}"/>
+  <autoFilter ref="A1:F80" xr:uid="{58D884C3-B977-47D3-B44D-AB1230B14EE3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>